<commit_message>
Update mwd and piling property draft codelists
</commit_message>
<xml_diff>
--- a/Draft Excel Codelists/mwd_properties.xlsx
+++ b/Draft Excel Codelists/mwd_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Draft Excel Codelists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FADCFBF-A3C7-5447-AF72-B8EA44D20B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D9FBE4-9276-8B4C-9A11-F6DE3969760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27820" yWindow="4900" windowWidth="27500" windowHeight="22180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11920" yWindow="4600" windowWidth="42380" windowHeight="25060" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="384">
   <si>
     <t>Description</t>
   </si>
@@ -789,45 +789,15 @@
     <t>Cross-sectional area of excavated borehole</t>
   </si>
   <si>
-    <t>Maximum Torque available on the drill rig</t>
-  </si>
-  <si>
-    <t>Maximum crowd available on the drill rig</t>
-  </si>
-  <si>
-    <t>Baseline torque pressure</t>
-  </si>
-  <si>
-    <t>Baseline crowd pressure</t>
-  </si>
-  <si>
-    <t>Crowd conversion coefficient</t>
-  </si>
-  <si>
-    <t>Maximum operating pressure of drill rig hydraulic system</t>
-  </si>
-  <si>
     <t>Hydraulic torque operating pressure</t>
   </si>
   <si>
     <t>Hydraulic crowd operating pressure</t>
   </si>
   <si>
-    <t>Maximum hydraulic motor displacement</t>
-  </si>
-  <si>
-    <t>Minimum hydraulic motor displacement</t>
-  </si>
-  <si>
     <t>Hydraulic fluid flow rate</t>
   </si>
   <si>
-    <t>Number of hydraulic motors</t>
-  </si>
-  <si>
-    <t>Gearcase reduction for each gear (n)</t>
-  </si>
-  <si>
     <t>Specific energy</t>
   </si>
   <si>
@@ -843,9 +813,6 @@
     <t>Soil-rock resistance</t>
   </si>
   <si>
-    <t>Ground Water Table</t>
-  </si>
-  <si>
     <t>Weight of drill rod or drill string</t>
   </si>
   <si>
@@ -858,9 +825,6 @@
     <t>penetration_rate</t>
   </si>
   <si>
-    <t>rotational_speed</t>
-  </si>
-  <si>
     <t>fluid_injection_volume_rate</t>
   </si>
   <si>
@@ -897,51 +861,18 @@
     <t>recorded_depth_increment</t>
   </si>
   <si>
-    <t>drill_bit_diameter</t>
-  </si>
-  <si>
     <t>excavated_borehole_area</t>
   </si>
   <si>
-    <t>max_torque_drill_rig</t>
-  </si>
-  <si>
-    <t>max_crowd_drill_rig</t>
-  </si>
-  <si>
-    <t>baseline_torque_pressure</t>
-  </si>
-  <si>
-    <t>baseline_crowd_pressure</t>
-  </si>
-  <si>
-    <t>crowd_conversion_coeff</t>
-  </si>
-  <si>
-    <t>max_operating_pressure_drill_rig</t>
-  </si>
-  <si>
     <t>hydraulic_torque_pressure</t>
   </si>
   <si>
     <t>hydraulic_crowd_pressure</t>
   </si>
   <si>
-    <t>max_hydraulic_motor_displacement</t>
-  </si>
-  <si>
-    <t>min_hydraulic_motor_displacement</t>
-  </si>
-  <si>
     <t>hydraulic_fluid_flow_rate</t>
   </si>
   <si>
-    <t>num_hydraulic_motors</t>
-  </si>
-  <si>
-    <t>gearcase_reduction</t>
-  </si>
-  <si>
     <t>specific_energy</t>
   </si>
   <si>
@@ -957,18 +888,12 @@
     <t>soil_rock_resistance</t>
   </si>
   <si>
-    <t>ground_water_table</t>
-  </si>
-  <si>
     <t>drill_rod_weight</t>
   </si>
   <si>
     <t xml:space="preserve">Measured time </t>
   </si>
   <si>
-    <t>Drill bit diameter</t>
-  </si>
-  <si>
     <t>Torque (in-lbs): The rotational force applied by the drill rig, measured in inch-pounds.</t>
   </si>
   <si>
@@ -996,48 +921,15 @@
     <t>Recorded depth increment (in, ft): The incremental depth recorded, usually after a certain operation or time interval, measured in inches or feet.</t>
   </si>
   <si>
-    <t>Drill bit diameter (in): The diameter of the drill bit, measured in inches.</t>
-  </si>
-  <si>
-    <t>Maximum Torque available on the drill rig (ft-lbs): The highest rotational force that can be applied by the drill rig, measured in foot-pounds.</t>
-  </si>
-  <si>
-    <t>Baseline torque pressure (psi): The standard operating pressure for torque application on the drill rig, measured in pounds per square inch.</t>
-  </si>
-  <si>
-    <t>Baseline crowd pressure (psi): The standard operating pressure for crowd force application on the drill rig, measured in pounds per square inch.</t>
-  </si>
-  <si>
-    <t>Crowd conversion coefficient (lbf/psi): The ratio of crowd force to the pressure applied, measured in pounds-force per square inch.</t>
-  </si>
-  <si>
-    <t>Maximum operating pressure of drill rig hydraulic system (psi): The highest pressure at which the drill rig's hydraulic system can operate, measured in pounds per square inch.</t>
-  </si>
-  <si>
-    <t>Maximum hydraulic motor displacement (in³/rev): The maximum volume displaced by the hydraulic motor per revolution, measured in cubic inches per revolution.</t>
-  </si>
-  <si>
-    <t>Minimum hydraulic motor displacement (in³/rev): The minimum volume displaced by the hydraulic motor per revolution, measured in cubic inches per revolution.</t>
-  </si>
-  <si>
     <t>Hydraulic fluid flow rate (in³/min): The flow rate of the hydraulic fluid, measured in cubic inches per minute.</t>
   </si>
   <si>
-    <t>Number of hydraulic motors (-): The count of hydraulic motors used in the drilling setup.</t>
-  </si>
-  <si>
-    <t>Gearcase reduction for each gear (n) (-): The gear reduction ratio in the gearcase for each gear, a unitless number.</t>
-  </si>
-  <si>
     <t>Drillability strength (psi)</t>
   </si>
   <si>
     <t>Specific energy (psi)</t>
   </si>
   <si>
-    <t>Ground Water Table Depth (ft)</t>
-  </si>
-  <si>
     <t>Somerton index (-)</t>
   </si>
   <si>
@@ -1089,51 +981,18 @@
     <t>AASHTO Designation: TP xxx-yy16</t>
   </si>
   <si>
-    <t>AASHTO Designation: TP xxx-yy17</t>
-  </si>
-  <si>
     <t>AASHTO Designation: TP xxx-yy18</t>
   </si>
   <si>
-    <t>AASHTO Designation: TP xxx-yy19</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy20</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy21</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy22</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy23</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy24</t>
-  </si>
-  <si>
     <t>AASHTO Designation: TP xxx-yy25</t>
   </si>
   <si>
     <t>AASHTO Designation: TP xxx-yy26</t>
   </si>
   <si>
-    <t>AASHTO Designation: TP xxx-yy27</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy28</t>
-  </si>
-  <si>
     <t>AASHTO Designation: TP xxx-yy29</t>
   </si>
   <si>
-    <t>AASHTO Designation: TP xxx-yy30</t>
-  </si>
-  <si>
-    <t>AASHTO Designation: TP xxx-yy31</t>
-  </si>
-  <si>
     <t>AASHTO Designation: TP xxx-yy32</t>
   </si>
   <si>
@@ -1149,9 +1008,6 @@
     <t>AASHTO Designation: TP xxx-yy36</t>
   </si>
   <si>
-    <t>AASHTO Designation: TP xxx-yy37</t>
-  </si>
-  <si>
     <t>AASHTO Designation: TP xxx-yy38</t>
   </si>
   <si>
@@ -1170,9 +1026,6 @@
     <t>True False Flag for when the drill rig stops (1,0)</t>
   </si>
   <si>
-    <t>torquetach</t>
-  </si>
-  <si>
     <t>torque Tach (%)</t>
   </si>
   <si>
@@ -1221,36 +1074,6 @@
     <t>Nvalue (-)</t>
   </si>
   <si>
-    <t>Data Capture Software</t>
-  </si>
-  <si>
-    <t>Indentier of the data processing software and version</t>
-  </si>
-  <si>
-    <t>drilling_activity_note</t>
-  </si>
-  <si>
-    <t>Drilling Activity Note</t>
-  </si>
-  <si>
-    <t>current_drilling_state</t>
-  </si>
-  <si>
-    <t>Current Drilling State</t>
-  </si>
-  <si>
-    <t>Make notes of things while drilling MWD, or transitioning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auger drilling, Mud rtotary, hollow stem, rock core. </t>
-  </si>
-  <si>
-    <t>data_capture_software</t>
-  </si>
-  <si>
-    <t>instrumentation_calibration_desc</t>
-  </si>
-  <si>
     <t>True False Flag for if this is a calibration test</t>
   </si>
   <si>
@@ -1314,30 +1137,9 @@
     <t>The number of the gear that is engaged</t>
   </si>
   <si>
-    <t>auger_od</t>
-  </si>
-  <si>
-    <t>Auger OD</t>
-  </si>
-  <si>
     <t>Fluid injection pressure (psi): The pressure at which drilling fluid is injected into the well.</t>
   </si>
   <si>
-    <t>Should be construction method drill rig tool info</t>
-  </si>
-  <si>
-    <t>core_</t>
-  </si>
-  <si>
-    <t>core_diameter</t>
-  </si>
-  <si>
-    <t>Diameter of the core</t>
-  </si>
-  <si>
-    <t>core diameter</t>
-  </si>
-  <si>
     <t>measurement parameter</t>
   </si>
   <si>
@@ -1353,9 +1155,6 @@
     <t>Total weight of the drill rod or drill string (lbf); increases as a new section Is added, Check that this is really total weight</t>
   </si>
   <si>
-    <t>Cross-sectional area of excavated borehole (in²): The cross-sectional area of the borehole cleared by the drill bit, measured in square inches. Assumed dein seukk vur suNWRWE IE or measured with caliper tool?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -1368,9 +1167,6 @@
     <t>Hydraulic torque operating pressure (psi): The pressure at which the hydraulic system operates to deliver torque, measured in pounds per square inch. Confirm that this is a value that changes while drilling or is an initial propoerty that does not change while drilling.</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum crowd available on the drill rig (lbf): The maximum downward force that can be exerted by the drill rig, measured in pounds-force. </t>
-  </si>
-  <si>
     <t>Injected fluid dynamic viscosity (lbf-s/ft²): The resistance of the injected fluid to flow, measured in pound-force seconds per square foot. Confirm that this is a value that changes while drilling or is an initial propoerty that does not change while drilling.</t>
   </si>
   <si>
@@ -1390,13 +1186,16 @@
   </si>
   <si>
     <t>Vibration (ft/s²): The rate of change of velocity per second of the drill string, measured in feet per second squared. Funny definition - vibration implies oscillation, not acceleration.</t>
+  </si>
+  <si>
+    <t>Cross-sectional area of excavated borehole (in²): The cross-sectional area of the borehole cleared by the drill bit, measured in square inches. Assumed from drill  biy diameter  or measured with caliper tool?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1489,15 +1288,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1508,12 +1300,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FF4472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDBE5F1"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1602,7 +1388,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1626,8 +1412,8 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1638,81 +1424,51 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1729,17 +1485,11 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1749,17 +1499,46 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1875,11 +1654,17 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1889,46 +1674,17 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1994,40 +1750,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H51" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:H51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H51">
-    <sortCondition ref="B1:B51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H34" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:H34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H34">
+    <sortCondition ref="B1:B34"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="9">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2863,1,FALSE)),"Not used","")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="12">
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2846,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D46" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:D46" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D33" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C2">
     <sortCondition ref="C1:C2"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="13">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2359,10 +2115,10 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>373</v>
+        <v>325</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>234</v>
@@ -2380,1225 +2136,845 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="27" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="84.6640625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="27" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="27"/>
+    <col min="1" max="1" width="7" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="84.6640625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="22" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2863,1,FALSE)),"Not used","")</f>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2890,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2847,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B2851,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2883,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2878,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2863,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2851,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B2852,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2850,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2853,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B2865,1,FALSE)),"Not used","")</f>
         <v>Not used</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>425</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>428</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="B12" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2870,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B2857,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2854,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B2855,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2860,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2884,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="G19" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2859,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2858,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2848,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2880,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2861,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2849,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2885,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2850,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2881,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2879,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>322</v>
-      </c>
-      <c r="E3" s="30" t="s">
+      <c r="D30" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="E30" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F30" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B2883,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>252</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>321</v>
-      </c>
-      <c r="E4" s="30" t="s">
+      <c r="G30" s="18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2884,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2846,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="E32" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2907,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>405</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>406</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>404</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>430</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>432</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>431</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2885,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>323</v>
-      </c>
-      <c r="E7" s="30" t="s">
+      <c r="F32" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2885,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2864,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>311</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="F33" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="23"/>
+    </row>
+    <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="str">
+        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2856,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E34" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B2868,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>416</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>417</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>418</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="32"/>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2905,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>398</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>399</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>401</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2903,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>394</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>395</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B2879,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>309</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>319</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2900,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>307</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>269</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>437</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B2895,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2904,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>397</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>400</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B2880,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>287</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>438</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2868,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>314</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B2869,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>427</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2867,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>313</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2870,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>315</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2893,C195,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>262</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>329</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2882,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>423</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>424</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="G22" s="32"/>
-    </row>
-    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2899,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>332</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="27" t="s">
+      <c r="F34" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="14" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="15" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B39" s="16" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2888,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>295</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>257</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2891,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>327</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2887,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>256</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>316</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="G28" s="27" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2872,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>279</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>444</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="27" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2882,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>443</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="27" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2889,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>325</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2886,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="27" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2881,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>320</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>409</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" s="27" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>283</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>308</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>317</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="27" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B2890,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>259</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>326</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B2892,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>328</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="27" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A38" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B2875,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>445</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G38" s="27" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B2865,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>272</v>
-      </c>
-      <c r="C39" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>312</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="27" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B2897,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>446</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F40" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B2878,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="C41" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="D41" s="31" t="s">
-        <v>318</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A42" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B2866,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>410</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>411</v>
-      </c>
-      <c r="D42" s="31" t="s">
-        <v>412</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="27" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" s="33" t="str">
-        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B2902,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>419</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>420</v>
-      </c>
-      <c r="D43" s="41" t="s">
-        <v>447</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G43" s="32"/>
-    </row>
-    <row r="44" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B2867,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>413</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>414</v>
-      </c>
-      <c r="D44" s="31" t="s">
-        <v>415</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B45,AssociatedElements!B$2:B2898,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>305</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>448</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B46,AssociatedElements!B$2:B2896,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>265</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>333</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="27" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B47,AssociatedElements!B$2:B2894,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>301</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="D47" s="31" t="s">
-        <v>331</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" s="27" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B48,AssociatedElements!B$2:B2901,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>374</v>
-      </c>
-      <c r="C48" s="31" t="s">
-        <v>375</v>
-      </c>
-      <c r="D48" s="31" t="s">
-        <v>376</v>
-      </c>
-      <c r="E48" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="F48" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="32"/>
-    </row>
-    <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B49,AssociatedElements!B$2:B2863,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="C49" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="E49" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="F49" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G49" s="27" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B50,AssociatedElements!B$2:B2902,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>421</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>378</v>
-      </c>
-      <c r="D50" s="38" t="s">
-        <v>449</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F50" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="32"/>
-    </row>
-    <row r="51" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A51" s="27" t="str">
-        <f>IF(ISNA(VLOOKUP(B51,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>280</v>
-      </c>
-      <c r="C51" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="D51" s="38" t="s">
-        <v>450</v>
-      </c>
-      <c r="E51" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F51" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="G51" s="27" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="14" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="15" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="16" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="20" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="39" t="s">
-        <v>439</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -3611,17 +2987,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E8BE39A-6790-4C87-932D-CBC46A1C9925}">
+          <x14:formula1>
+            <xm:f>Lists!$C$2:$C$187</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F16</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$178</xm:f>
           </x14:formula1>
-          <xm:sqref>F28:F32 F34:F45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E8BE39A-6790-4C87-932D-CBC46A1C9925}">
-          <x14:formula1>
-            <xm:f>Lists!$C$2:$C$187</xm:f>
-          </x14:formula1>
-          <xm:sqref>F33 F3:F27</xm:sqref>
+          <xm:sqref>F17:F28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3632,11 +3008,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3663,678 +3039,467 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D2" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D3" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D4" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
+        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B6" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D6" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D7" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D8" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B9" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D9" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D10" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D11" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D12" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D13" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B14" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D14" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B15" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D15" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B16" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D16" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B17" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D17" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D18" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B19" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D19" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B20" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D20" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B21" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D21" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B22" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D22" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B23" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D23" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B24" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D24" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B25" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D25" t="s">
-        <v>408</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B26" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D26" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B27" t="s">
-        <v>295</v>
+        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>326</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D27" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B28" t="s">
-        <v>296</v>
+        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>362</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D28" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B29" t="s">
-        <v>297</v>
+        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>346</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>407</v>
+        <v>348</v>
       </c>
       <c r="D29" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B30" t="s">
-        <v>298</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D30" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B31" t="s">
-        <v>299</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D31" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B32" t="s">
-        <v>300</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D32" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B33" t="s">
-        <v>301</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D33" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B34" t="s">
-        <v>302</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D34" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B35" t="s">
-        <v>303</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D35" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B36" t="s">
-        <v>304</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D36" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B37" t="s">
-        <v>305</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D37" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B38" t="s">
-        <v>306</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D38" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B39" t="s">
-        <v>307</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D39" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D40" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D41" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>402</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D42" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" t="str">
-        <f>IF(ISNA(VLOOKUP(B43,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D43" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" t="str">
-        <f>IF(ISNA(VLOOKUP(B44,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D44" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="str">
-        <f>IF(ISNA(VLOOKUP(B45,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D45" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="str">
-        <f>IF(ISNA(VLOOKUP(B46,Definitions!B$3:B$1850,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>405</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="D46" t="s">
-        <v>408</v>
-      </c>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="30" t="str">
+        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>357</v>
+      </c>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="30" t="str">
+        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>351</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="30" t="str">
+        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="30" t="str">
+        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1833,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="33"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C2">
@@ -5614,77 +4779,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>379</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>380</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>385</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>386</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>387</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>388</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>389</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>390</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>391</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>392</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>393</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>